<commit_message>
bug fixed and reproduced Raven tests
</commit_message>
<xml_diff>
--- a/scoring/tests/Raven/Raven9A_test_1.xlsx
+++ b/scoring/tests/Raven/Raven9A_test_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="question_answers" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="outputs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="question_answers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="outputs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -440,7 +440,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -760,7 +760,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -810,7 +810,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -850,7 +850,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -860,7 +860,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -890,7 +890,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -925,7 +925,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -995,19 +995,7 @@
           <t>report</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>زیر متوسط</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+      <c r="B6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>